<commit_message>
started ckdtree algorithm implementation
</commit_message>
<xml_diff>
--- a/exactpoints.xlsx
+++ b/exactpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpiernicki\Desktop\code\Pairing_points_algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E55878-BD1C-40B1-954F-F7DB3EA77011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B7D62D-C421-4BF6-BBED-6095C6CB6AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{A4A5F9A4-5C1D-4C0B-9E98-2027115D1FB9}"/>
+    <workbookView xWindow="-14850" yWindow="7890" windowWidth="21600" windowHeight="11385" xr2:uid="{A4A5F9A4-5C1D-4C0B-9E98-2027115D1FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD23"/>
+      <selection activeCell="F2" sqref="F2:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>